<commit_message>
Descargue hasta Lorenzo Vera - 26/6
</commit_message>
<xml_diff>
--- a/Desafios/03/Pair Programming.xlsx
+++ b/Desafios/03/Pair Programming.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\Bootcamp 71241\Desafios\03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UdeSA\AppData\Development\Bootcamp-71241\Desafios\03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E691887D-B1CD-4AE0-BC33-B28D29E79D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Tareas de Pair Programming - Práctico 3</t>
   </si>
@@ -120,9 +119,6 @@
     <t>Sindy González</t>
   </si>
   <si>
-    <t>Matías Villalba</t>
-  </si>
-  <si>
     <t>Matías Heredia</t>
   </si>
   <si>
@@ -139,13 +135,19 @@
   </si>
   <si>
     <t>Román Ledesma</t>
+  </si>
+  <si>
+    <t>Matias Villalba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Agustin Giuli participo ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +309,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -314,9 +319,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -598,28 +600,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="36.6" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="79.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="2:5" ht="36.6" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -630,29 +633,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -663,51 +666,51 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -718,18 +721,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -740,108 +743,104 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B14" s="3">
         <v>11</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B15" s="3">
         <v>12</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
       <c r="B16" s="3">
         <v>13</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
       <c r="B17" s="3">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B21" s="3">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="3">
-        <v>15</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="3">
-        <v>16</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="3">
-        <v>17</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="3">
-        <v>18</v>
-      </c>
-      <c r="C21" s="5"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
       <c r="B22" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="3">
-        <v>20</v>
-      </c>
-      <c r="C23" s="5"/>
+    <row r="23" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+      <c r="B23" s="7"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Correccion - Me quede en Martin Desch y rodriguez
</commit_message>
<xml_diff>
--- a/Desafios/03/Pair Programming.xlsx
+++ b/Desafios/03/Pair Programming.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UdeSA\AppData\Development\Bootcamp-71241\Desafios\03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\Bootcamp 71241\Desafios\03\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6143C629-E322-4AF2-93A5-41D3DDF01E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -146,8 +147,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -320,6 +321,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,29 +604,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="36.6" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="5" width="79.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="5" max="5" width="79.33203125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="36.6" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="1" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="11"/>
     </row>
-    <row r="3" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="3" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,7 +637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="4" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -644,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="5" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -655,7 +659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="6" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -666,7 +670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="7" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -677,7 +681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="8" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -688,7 +692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="9" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -699,7 +703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="10" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -710,7 +714,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="11" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>8</v>
       </c>
@@ -721,7 +725,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="12" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>9</v>
       </c>
@@ -732,7 +736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="13" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -743,7 +747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="14" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>11</v>
       </c>
@@ -754,7 +758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+    <row r="15" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>12</v>
       </c>
@@ -764,8 +768,11 @@
       <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="36.6" customHeight="1" thickBot="1">
+      <c r="E15" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>13</v>
       </c>
@@ -775,11 +782,11 @@
       <c r="D16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+    <row r="17" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>15</v>
       </c>
@@ -790,7 +797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+    <row r="18" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>16</v>
       </c>
@@ -801,7 +808,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+    <row r="19" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>17</v>
       </c>
@@ -812,7 +819,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+    <row r="20" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <v>18</v>
       </c>
@@ -821,7 +828,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+    <row r="21" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>19</v>
       </c>
@@ -830,14 +837,14 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+    <row r="22" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <v>20</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="2:4" ht="36.6" customHeight="1" thickBot="1">
+    <row r="23" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>

</xml_diff>